<commit_message>
created and read data from products and order details
</commit_message>
<xml_diff>
--- a/Connected Office Web Application_User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Connected Office Web Application_User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nttlimited-my.sharepoint.com/personal/jacqui_muller_dimensiondata_com/Documents/NWU/2023 CMPG323/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntima\OneDrive\Desktop\CMPG323-Projects\CMPG323-Project4-31967000\Connected Office Web Application_User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5546F926-6C85-4EAE-890A-D0833008B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B224C2EE-D72C-413C-83C8-0FBC3DD6E173}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -383,7 +382,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -729,7 +728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -990,7 +989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1712,7 +1711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1947,7 +1946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>